<commit_message>
Change category ‘PreSeizure’ to ‘PeriIctalSignals’
Change category ‘PreSeizure’ to ‘PeriIctalSignals’
</commit_message>
<xml_diff>
--- a/Incorrect_prediction_info_SegAsUnits_2.xlsx
+++ b/Incorrect_prediction_info_SegAsUnits_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Imperial\Spring\Project\GitKraken\EEG_ChenYANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122828A6-E0FA-4773-9A69-3E77E64B5A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772BF055-6956-4AF6-A4EE-8293421D94D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="7">
   <si>
     <t>Segment index</t>
   </si>
@@ -28,13 +28,10 @@
     <t>True value</t>
   </si>
   <si>
-    <t>PreSeizure</t>
+    <t>PeriIctalSignals</t>
   </si>
   <si>
     <t>Seizure</t>
-  </si>
-  <si>
-    <t>AfterSeizure</t>
   </si>
   <si>
     <t>#ch pre as Seisure</t>
@@ -43,7 +40,7 @@
     <t>#ch pre as NonSeisure</t>
   </si>
   <si>
-    <t>#ch pre as PreSeisure</t>
+    <t>#ch pre as PeriIctalSignals</t>
   </si>
 </sst>
 </file>
@@ -117,17 +114,7 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.2524284979841438E-2"/>
-          <c:y val="3.2128514056224897E-2"/>
-          <c:w val="0.92823172876586302"/>
-          <c:h val="0.81977864212756535"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -171,184 +158,214 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$56</c:f>
+              <c:f>Sheet1!$A$2:$A$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="14">
                   <c:v>111</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="15">
                   <c:v>112</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
                   <c:v>113</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
                   <c:v>114</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="18">
                   <c:v>115</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="19">
                   <c:v>116</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="20">
                   <c:v>117</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="21">
                   <c:v>118</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="22">
                   <c:v>119</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="23">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="24">
                   <c:v>121</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
                   <c:v>122</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="26">
                   <c:v>123</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="28">
                   <c:v>125</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="29">
                   <c:v>126</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="30">
                   <c:v>127</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="31">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="32">
                   <c:v>129</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="33">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="34">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="35">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="36">
                   <c:v>133</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="37">
                   <c:v>134</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="38">
                   <c:v>135</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="39">
                   <c:v>136</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="40">
                   <c:v>137</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="41">
                   <c:v>138</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="42">
                   <c:v>139</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="43">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="44">
                   <c:v>141</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="45">
                   <c:v>142</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="46">
                   <c:v>143</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="47">
                   <c:v>144</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="48">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="49">
                   <c:v>146</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="50">
                   <c:v>147</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="51">
                   <c:v>148</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="52">
                   <c:v>149</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="53">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="54">
                   <c:v>151</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="55">
                   <c:v>152</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="56">
                   <c:v>153</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="57">
                   <c:v>154</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="58">
                   <c:v>155</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="59">
                   <c:v>156</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="60">
                   <c:v>157</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="61">
                   <c:v>158</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="62">
                   <c:v>159</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="63">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="64">
                   <c:v>161</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$56</c:f>
+              <c:f>Sheet1!$C$2:$C$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -395,52 +412,52 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>30</c:v>
@@ -449,70 +466,100 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,7 +567,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1742-403E-8672-E515D7ED1148}"/>
+              <c16:uniqueId val="{00000000-C082-4D71-B7CB-B5223B880D4C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -564,348 +611,408 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$56</c:f>
+              <c:f>Sheet1!$A$2:$A$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="14">
                   <c:v>111</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="15">
                   <c:v>112</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
                   <c:v>113</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
                   <c:v>114</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="18">
                   <c:v>115</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="19">
                   <c:v>116</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="20">
                   <c:v>117</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="21">
                   <c:v>118</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="22">
                   <c:v>119</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="23">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="24">
                   <c:v>121</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
                   <c:v>122</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="26">
                   <c:v>123</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="28">
                   <c:v>125</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="29">
                   <c:v>126</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="30">
                   <c:v>127</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="31">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="32">
                   <c:v>129</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="33">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="34">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="35">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="36">
                   <c:v>133</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="37">
                   <c:v>134</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="38">
                   <c:v>135</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="39">
                   <c:v>136</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="40">
                   <c:v>137</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="41">
                   <c:v>138</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="42">
                   <c:v>139</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="43">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="44">
                   <c:v>141</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="45">
                   <c:v>142</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="46">
                   <c:v>143</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="47">
                   <c:v>144</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="48">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="49">
                   <c:v>146</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="50">
                   <c:v>147</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="51">
                   <c:v>148</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="52">
                   <c:v>149</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="53">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="54">
                   <c:v>151</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="55">
                   <c:v>152</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="56">
                   <c:v>153</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="57">
                   <c:v>154</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="58">
                   <c:v>155</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="59">
                   <c:v>156</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="60">
                   <c:v>157</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="61">
                   <c:v>158</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="62">
                   <c:v>159</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="63">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="64">
                   <c:v>161</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$56</c:f>
+              <c:f>Sheet1!$D$2:$D$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="40">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="35">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="49">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>17</c:v>
+                <c:pt idx="55">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -913,7 +1020,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1742-403E-8672-E515D7ED1148}"/>
+              <c16:uniqueId val="{00000001-C082-4D71-B7CB-B5223B880D4C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -926,7 +1033,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>#ch pre as PreSeisure</c:v>
+                  <c:v>#ch pre as PeriIctalSignals</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -957,255 +1064,285 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$56</c:f>
+              <c:f>Sheet1!$A$2:$A$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="14">
                   <c:v>111</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="15">
                   <c:v>112</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
                   <c:v>113</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
                   <c:v>114</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="18">
                   <c:v>115</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="19">
                   <c:v>116</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="20">
                   <c:v>117</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="21">
                   <c:v>118</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="22">
                   <c:v>119</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="23">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="24">
                   <c:v>121</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
                   <c:v>122</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="26">
                   <c:v>123</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="28">
                   <c:v>125</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="29">
                   <c:v>126</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="30">
                   <c:v>127</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="31">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="32">
                   <c:v>129</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="33">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="34">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="35">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="36">
                   <c:v>133</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="37">
                   <c:v>134</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="38">
                   <c:v>135</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="39">
                   <c:v>136</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="40">
                   <c:v>137</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="41">
                   <c:v>138</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="42">
                   <c:v>139</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="43">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="44">
                   <c:v>141</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="45">
                   <c:v>142</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="46">
                   <c:v>143</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="47">
                   <c:v>144</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="48">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="49">
                   <c:v>146</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="50">
                   <c:v>147</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="51">
                   <c:v>148</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="52">
                   <c:v>149</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="53">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="54">
                   <c:v>151</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="55">
                   <c:v>152</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="56">
                   <c:v>153</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="57">
                   <c:v>154</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="58">
                   <c:v>155</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="59">
                   <c:v>156</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="60">
                   <c:v>157</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="61">
                   <c:v>158</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="62">
                   <c:v>159</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="63">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="64">
                   <c:v>161</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$56</c:f>
+              <c:f>Sheet1!$E$2:$E$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -1238,67 +1375,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="38">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1306,7 +1473,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1742-403E-8672-E515D7ED1148}"/>
+              <c16:uniqueId val="{00000002-C082-4D71-B7CB-B5223B880D4C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1318,15 +1485,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1879073615"/>
-        <c:axId val="1879093295"/>
+        <c:axId val="598161632"/>
+        <c:axId val="598185632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1879073615"/>
+        <c:axId val="598161632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="164"/>
-          <c:min val="110"/>
+          <c:max val="161"/>
+          <c:min val="97"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1381,12 +1548,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1879093295"/>
+        <c:crossAx val="598185632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1879093295"/>
+        <c:axId val="598185632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,7 +1610,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1879073615"/>
+        <c:crossAx val="598161632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2090,23 +2257,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>845820</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8806B49A-9A98-5387-82DF-FA5B1D154FCF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7060BB3E-211F-1611-97D6-516860ED25BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2444,19 +2611,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -2467,18 +2634,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -2487,15 +2654,15 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E2">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -2504,15 +2671,15 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -2521,15 +2688,15 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -2538,15 +2705,15 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -2555,15 +2722,15 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E6">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -2572,15 +2739,15 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E7">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -2589,15 +2756,15 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -2606,15 +2773,15 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -2623,15 +2790,15 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E10">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -2640,15 +2807,15 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E11">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -2657,15 +2824,15 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -2674,15 +2841,15 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -2691,15 +2858,15 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -2708,15 +2875,15 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -2725,24 +2892,24 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E17">
         <v>6</v>
@@ -2750,152 +2917,152 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>18</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
       <c r="C24">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -2903,16 +3070,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
       <c r="C27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2920,16 +3087,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2937,7 +3104,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
@@ -2954,16 +3121,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -2971,7 +3138,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -2988,16 +3155,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -3005,7 +3172,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -3022,7 +3189,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -3039,16 +3206,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="C35">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -3056,365 +3223,534 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E37">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
         <v>4</v>
       </c>
-      <c r="C38">
-        <v>8</v>
-      </c>
-      <c r="D38">
-        <v>20</v>
-      </c>
       <c r="E38">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D39">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E41">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
         <v>8</v>
       </c>
-      <c r="D42">
-        <v>17</v>
-      </c>
       <c r="E42">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E45">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
         <v>6</v>
       </c>
-      <c r="D46">
-        <v>23</v>
-      </c>
       <c r="E46">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E49">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E50">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C51">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E51">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C52">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E52">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E54">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C56">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E56">
-        <v>8</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>152</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>153</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>30</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>154</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>30</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>155</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>29</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>156</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>30</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>157</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>30</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>158</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>30</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>159</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>30</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>160</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>30</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>161</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>19</v>
+      </c>
+      <c r="E66">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>